<commit_message>
editing item in list
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">placa de vídeo rx 5500</t>
   </si>
   <si>
-    <t xml:space="preserve">ddr4 16gb memória</t>
+    <t xml:space="preserve">memória ram ddr4 16gb</t>
   </si>
   <si>
     <t xml:space="preserve">ssd kingston 512gb</t>
@@ -152,10 +152,10 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.38"/>
   </cols>

</xml_diff>

<commit_message>
editing list of items
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -22,37 +22,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t xml:space="preserve">processador i5 10 geracao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">placa mãe asus tuf gaming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">placa de vídeo rx 5500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">memória ram ddr4 16gb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssd kingston 512gb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fonte corsair 550w</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gabinete cooler master</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teclado corsair k70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mouse logitech g502 hero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">headset jbl quantum 100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monitor acer 100hz</t>
+    <t xml:space="preserve">Processador gamer Intel Core i5-10400F BX8070110400F de 6 núcleos e 4.3GHz de frequência</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placa Mãe Asus Para Intel 1700 Z690 Plus D4 Tuf 4ddr4 Atx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placa De Video Mancer Rx 5500 Xt Streaky, 8gb, Gddr6 128 Bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memória RAM NB BLACK color preto 16GB 1 UP Gamer UP3200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disco Sólido Interno Kingston Skc600/512g 512gb Preto Cor Preto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fonte de alimentação para PC Corsair CV Series CV550 550W black 100V/240V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabinete Gamer Cooler Master Elite 300 Lateral Vidro Preto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teclado Corsair K55 Rgb Multicolor Led</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouse Logitech G G Series G502 Hero preto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitor Acer 21.5 Zero Frame Radeon Hdmi Ea220q Hbi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headset Gamer Para Consoles E Pc Driver 40mm Quantum 100 Preto Jbl</t>
   </si>
 </sst>
 </file>
@@ -152,12 +152,13 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="78.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>